<commit_message>
hame actiona be joz yeseria
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Ap\Group05\Group-05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE6AA6F-18DF-4094-B15B-D00BFC1E3129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D2F075-D007-4EFD-99A7-16744C46FDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{567B7C76-1CED-4D0D-B579-74A0634403A6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{567B7C76-1CED-4D0D-B579-74A0634403A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Skellige" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Skellige</t>
   </si>
   <si>
-    <t>در دور سوم بازی دو کارت رندوم از قبرستان اضافه می شود</t>
-  </si>
-  <si>
     <t>Mardoeme</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>در ردیف دوم قرار میگیرد و هر کارت مشابه خود را که در hand یا deck قرار دارد به میز می آورد</t>
   </si>
   <si>
-    <t>Iorveth</t>
-  </si>
-  <si>
     <t>Yaevinn</t>
   </si>
   <si>
@@ -757,6 +751,12 @@
   </si>
   <si>
     <t>Zoltan Chivay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2W</t>
   </si>
 </sst>
 </file>
@@ -1190,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2282DC8-EBD1-4E62-A2B3-958FFA21430E}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -1207,207 +1207,207 @@
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>1</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21">
       <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D466120D-0D08-489C-8741-6BBE850FC091}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -1434,194 +1434,194 @@
   <sheetData>
     <row r="1" spans="1:3" s="8" customFormat="1">
       <c r="A1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="11" t="s">
-        <v>52</v>
+        <v>239</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="23">
       <c r="A8" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="23">
       <c r="A16" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="23">
       <c r="A17" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="23">
       <c r="A18" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1656,285 +1656,285 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26">
       <c r="A1" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="21">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="21">
       <c r="A7" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="21">
       <c r="A10" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" ht="21">
       <c r="A15" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="21">
       <c r="A16" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="21">
       <c r="A19" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="21">
       <c r="A20" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1958,341 +1958,341 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="26">
       <c r="A2" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="26">
       <c r="A4" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="26">
       <c r="A6" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="26">
       <c r="A16" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="26">
       <c r="A17" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="26">
       <c r="A22" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="26">
       <c r="A27" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2316,365 +2316,365 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" ht="21">
       <c r="A25" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2698,242 +2698,242 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="23">
       <c r="A8" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" ht="23">
       <c r="A14" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="23">
       <c r="A17" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" ht="23">
       <c r="A21" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>

</xml_diff>